<commit_message>
Kavramsal tasarım raporu güncellendi
</commit_message>
<xml_diff>
--- a/DOCUMENT/PAPERS/İş zaman çizelgesi.xlsx
+++ b/DOCUMENT/PAPERS/İş zaman çizelgesi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre\kusbegi-teknofest\DOCUMENT\PAPERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFFB52F4-5E29-4458-8A2C-EDE0D90076BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076E3387-CD58-48C5-9801-5F6B30250DA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFD61A54-3209-43D0-9AF8-1F37F7D36D91}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>GÖREVLER</t>
   </si>
@@ -74,13 +74,16 @@
   <si>
     <t>Gerekli yazılımsal ayarlamaların tamamlanması
 ve son ürüne ulaşma</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +123,23 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -153,7 +173,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -165,6 +185,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="İyi" xfId="1" builtinId="26"/>
@@ -484,7 +508,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +525,7 @@
     <col min="18" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" customWidth="1"/>
     <col min="26" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -591,18 +615,22 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:28" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -610,22 +638,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -649,12 +683,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>

</xml_diff>